<commit_message>
[fix][asset] Fix asset bug to upload asset
</commit_message>
<xml_diff>
--- a/api/template/network_template.xlsx
+++ b/api/template/network_template.xlsx
@@ -10,7 +10,7 @@
     <sheet name="network" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">network!$A$1:$P$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">network!$A$1:$Q$78</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>机柜</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>设备厂商</t>
+  </si>
+  <si>
+    <t>设备类型</t>
   </si>
   <si>
     <t>设备型号</t>
@@ -1075,28 +1078,28 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:R68"/>
+  <dimension ref="A1:S68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="2" width="10.625" style="2" customWidth="1"/>
-    <col min="3" max="10" width="20.625" style="2" customWidth="1"/>
-    <col min="11" max="11" width="15.625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="20.625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="10.625" style="2" customWidth="1"/>
-    <col min="14" max="16" width="15.625" style="2" customWidth="1"/>
-    <col min="17" max="17" width="10.625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="30.625" style="2" customWidth="1"/>
-    <col min="19" max="16384" width="9" style="1"/>
+    <col min="3" max="11" width="20.625" style="2" customWidth="1"/>
+    <col min="12" max="12" width="15.625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="20.625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="10.625" style="2" customWidth="1"/>
+    <col min="15" max="17" width="15.625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="10.625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="30.625" style="2" customWidth="1"/>
+    <col min="20" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:18">
+    <row r="1" ht="15.75" spans="1:19">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1109,7 +1112,7 @@
       <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
@@ -1151,8 +1154,11 @@
       <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" s="1" customFormat="1" spans="1:18">
+      <c r="S1" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:19">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1169,10 +1175,11 @@
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
-      <c r="Q2" s="2"/>
+      <c r="Q2" s="5"/>
       <c r="R2" s="2"/>
-    </row>
-    <row r="3" s="1" customFormat="1" spans="1:18">
+      <c r="S2" s="2"/>
+    </row>
+    <row r="3" s="1" customFormat="1" spans="1:19">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1191,8 +1198,9 @@
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
-    </row>
-    <row r="4" s="1" customFormat="1" spans="1:18">
+      <c r="S3" s="2"/>
+    </row>
+    <row r="4" s="1" customFormat="1" spans="1:19">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1211,8 +1219,9 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
-    </row>
-    <row r="5" s="1" customFormat="1" spans="1:18">
+      <c r="S4" s="2"/>
+    </row>
+    <row r="5" s="1" customFormat="1" spans="1:19">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1231,8 +1240,9 @@
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
-    </row>
-    <row r="6" s="1" customFormat="1" spans="1:18">
+      <c r="S5" s="2"/>
+    </row>
+    <row r="6" s="1" customFormat="1" spans="1:19">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1251,8 +1261,9 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="1:18">
+      <c r="S6" s="2"/>
+    </row>
+    <row r="7" s="1" customFormat="1" spans="1:19">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1271,8 +1282,9 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
-    </row>
-    <row r="8" s="1" customFormat="1" spans="1:18">
+      <c r="S7" s="2"/>
+    </row>
+    <row r="8" s="1" customFormat="1" spans="1:19">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1291,8 +1303,9 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
-    </row>
-    <row r="9" s="1" customFormat="1" spans="1:18">
+      <c r="S8" s="2"/>
+    </row>
+    <row r="9" s="1" customFormat="1" spans="1:19">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1311,8 +1324,9 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
-    </row>
-    <row r="10" s="1" customFormat="1" spans="1:18">
+      <c r="S9" s="2"/>
+    </row>
+    <row r="10" s="1" customFormat="1" spans="1:19">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1331,8 +1345,9 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
-    </row>
-    <row r="11" s="1" customFormat="1" spans="1:18">
+      <c r="S10" s="2"/>
+    </row>
+    <row r="11" s="1" customFormat="1" spans="1:19">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1351,8 +1366,9 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
-    </row>
-    <row r="12" s="1" customFormat="1" spans="1:18">
+      <c r="S11" s="2"/>
+    </row>
+    <row r="12" s="1" customFormat="1" spans="1:19">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1371,8 +1387,9 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
-    </row>
-    <row r="13" s="1" customFormat="1" spans="1:18">
+      <c r="S12" s="2"/>
+    </row>
+    <row r="13" s="1" customFormat="1" spans="1:19">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1391,8 +1408,9 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
-    </row>
-    <row r="14" s="1" customFormat="1" spans="1:18">
+      <c r="S13" s="2"/>
+    </row>
+    <row r="14" s="1" customFormat="1" spans="1:19">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1411,8 +1429,9 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
-    </row>
-    <row r="15" s="1" customFormat="1" spans="1:18">
+      <c r="S14" s="2"/>
+    </row>
+    <row r="15" s="1" customFormat="1" spans="1:19">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1431,8 +1450,9 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
-    </row>
-    <row r="16" s="1" customFormat="1" spans="1:18">
+      <c r="S15" s="2"/>
+    </row>
+    <row r="16" s="1" customFormat="1" spans="1:19">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1451,8 +1471,9 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
-    </row>
-    <row r="17" s="1" customFormat="1" spans="1:18">
+      <c r="S16" s="2"/>
+    </row>
+    <row r="17" s="1" customFormat="1" spans="1:19">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1471,8 +1492,9 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
-    </row>
-    <row r="18" s="1" customFormat="1" spans="1:18">
+      <c r="S17" s="2"/>
+    </row>
+    <row r="18" s="1" customFormat="1" spans="1:19">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1491,8 +1513,9 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
-    </row>
-    <row r="19" s="1" customFormat="1" spans="1:18">
+      <c r="S18" s="2"/>
+    </row>
+    <row r="19" s="1" customFormat="1" spans="1:19">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1511,8 +1534,9 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
-    </row>
-    <row r="20" s="1" customFormat="1" spans="1:18">
+      <c r="S19" s="2"/>
+    </row>
+    <row r="20" s="1" customFormat="1" spans="1:19">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1531,8 +1555,9 @@
       <c r="P20" s="2"/>
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
-    </row>
-    <row r="21" s="1" customFormat="1" spans="1:18">
+      <c r="S20" s="2"/>
+    </row>
+    <row r="21" s="1" customFormat="1" spans="1:19">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1551,8 +1576,9 @@
       <c r="P21" s="2"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
-    </row>
-    <row r="22" s="1" customFormat="1" spans="1:18">
+      <c r="S21" s="2"/>
+    </row>
+    <row r="22" s="1" customFormat="1" spans="1:19">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1571,8 +1597,9 @@
       <c r="P22" s="2"/>
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
-    </row>
-    <row r="23" s="1" customFormat="1" spans="1:18">
+      <c r="S22" s="2"/>
+    </row>
+    <row r="23" s="1" customFormat="1" spans="1:19">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1591,8 +1618,9 @@
       <c r="P23" s="2"/>
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
-    </row>
-    <row r="24" s="1" customFormat="1" spans="1:18">
+      <c r="S23" s="2"/>
+    </row>
+    <row r="24" s="1" customFormat="1" spans="1:19">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1611,8 +1639,9 @@
       <c r="P24" s="2"/>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
-    </row>
-    <row r="25" s="1" customFormat="1" spans="1:18">
+      <c r="S24" s="2"/>
+    </row>
+    <row r="25" s="1" customFormat="1" spans="1:19">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1631,8 +1660,9 @@
       <c r="P25" s="2"/>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
-    </row>
-    <row r="26" s="1" customFormat="1" spans="1:18">
+      <c r="S25" s="2"/>
+    </row>
+    <row r="26" s="1" customFormat="1" spans="1:19">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1651,8 +1681,9 @@
       <c r="P26" s="2"/>
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
-    </row>
-    <row r="27" s="1" customFormat="1" spans="1:18">
+      <c r="S26" s="2"/>
+    </row>
+    <row r="27" s="1" customFormat="1" spans="1:19">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1671,8 +1702,9 @@
       <c r="P27" s="2"/>
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
-    </row>
-    <row r="28" s="1" customFormat="1" spans="1:18">
+      <c r="S27" s="2"/>
+    </row>
+    <row r="28" s="1" customFormat="1" spans="1:19">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1691,8 +1723,9 @@
       <c r="P28" s="2"/>
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
-    </row>
-    <row r="29" s="1" customFormat="1" spans="1:18">
+      <c r="S28" s="2"/>
+    </row>
+    <row r="29" s="1" customFormat="1" spans="1:19">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1711,8 +1744,9 @@
       <c r="P29" s="2"/>
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
-    </row>
-    <row r="30" s="1" customFormat="1" spans="1:18">
+      <c r="S29" s="2"/>
+    </row>
+    <row r="30" s="1" customFormat="1" spans="1:19">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1731,8 +1765,9 @@
       <c r="P30" s="2"/>
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
-    </row>
-    <row r="31" s="1" customFormat="1" spans="1:18">
+      <c r="S30" s="2"/>
+    </row>
+    <row r="31" s="1" customFormat="1" spans="1:19">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1751,8 +1786,9 @@
       <c r="P31" s="2"/>
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
-    </row>
-    <row r="32" s="1" customFormat="1" spans="1:18">
+      <c r="S31" s="2"/>
+    </row>
+    <row r="32" s="1" customFormat="1" spans="1:19">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1771,8 +1807,9 @@
       <c r="P32" s="2"/>
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
-    </row>
-    <row r="33" s="1" customFormat="1" spans="1:18">
+      <c r="S32" s="2"/>
+    </row>
+    <row r="33" s="1" customFormat="1" spans="1:19">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1791,8 +1828,9 @@
       <c r="P33" s="2"/>
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
-    </row>
-    <row r="34" s="1" customFormat="1" spans="1:18">
+      <c r="S33" s="2"/>
+    </row>
+    <row r="34" s="1" customFormat="1" spans="1:19">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1811,8 +1849,9 @@
       <c r="P34" s="2"/>
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
-    </row>
-    <row r="35" s="1" customFormat="1" spans="1:18">
+      <c r="S34" s="2"/>
+    </row>
+    <row r="35" s="1" customFormat="1" spans="1:19">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1831,8 +1870,9 @@
       <c r="P35" s="2"/>
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
-    </row>
-    <row r="36" s="1" customFormat="1" spans="1:18">
+      <c r="S35" s="2"/>
+    </row>
+    <row r="36" s="1" customFormat="1" spans="1:19">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1851,8 +1891,9 @@
       <c r="P36" s="2"/>
       <c r="Q36" s="2"/>
       <c r="R36" s="2"/>
-    </row>
-    <row r="37" s="1" customFormat="1" spans="1:18">
+      <c r="S36" s="2"/>
+    </row>
+    <row r="37" s="1" customFormat="1" spans="1:19">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1871,8 +1912,9 @@
       <c r="P37" s="2"/>
       <c r="Q37" s="2"/>
       <c r="R37" s="2"/>
-    </row>
-    <row r="38" s="1" customFormat="1" spans="1:18">
+      <c r="S37" s="2"/>
+    </row>
+    <row r="38" s="1" customFormat="1" spans="1:19">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1891,8 +1933,9 @@
       <c r="P38" s="2"/>
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
-    </row>
-    <row r="39" s="1" customFormat="1" spans="1:18">
+      <c r="S38" s="2"/>
+    </row>
+    <row r="39" s="1" customFormat="1" spans="1:19">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1911,8 +1954,9 @@
       <c r="P39" s="2"/>
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
-    </row>
-    <row r="40" s="1" customFormat="1" spans="1:18">
+      <c r="S39" s="2"/>
+    </row>
+    <row r="40" s="1" customFormat="1" spans="1:19">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1931,8 +1975,9 @@
       <c r="P40" s="2"/>
       <c r="Q40" s="2"/>
       <c r="R40" s="2"/>
-    </row>
-    <row r="41" s="1" customFormat="1" spans="1:18">
+      <c r="S40" s="2"/>
+    </row>
+    <row r="41" s="1" customFormat="1" spans="1:19">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1951,8 +1996,9 @@
       <c r="P41" s="2"/>
       <c r="Q41" s="2"/>
       <c r="R41" s="2"/>
-    </row>
-    <row r="42" s="1" customFormat="1" spans="1:18">
+      <c r="S41" s="2"/>
+    </row>
+    <row r="42" s="1" customFormat="1" spans="1:19">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -1971,8 +2017,9 @@
       <c r="P42" s="2"/>
       <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
-    </row>
-    <row r="43" s="1" customFormat="1" spans="1:18">
+      <c r="S42" s="2"/>
+    </row>
+    <row r="43" s="1" customFormat="1" spans="1:19">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -1991,8 +2038,9 @@
       <c r="P43" s="2"/>
       <c r="Q43" s="2"/>
       <c r="R43" s="2"/>
-    </row>
-    <row r="44" s="1" customFormat="1" spans="1:18">
+      <c r="S43" s="2"/>
+    </row>
+    <row r="44" s="1" customFormat="1" spans="1:19">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -2011,8 +2059,9 @@
       <c r="P44" s="2"/>
       <c r="Q44" s="2"/>
       <c r="R44" s="2"/>
-    </row>
-    <row r="45" s="1" customFormat="1" spans="1:18">
+      <c r="S44" s="2"/>
+    </row>
+    <row r="45" s="1" customFormat="1" spans="1:19">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -2031,8 +2080,9 @@
       <c r="P45" s="2"/>
       <c r="Q45" s="2"/>
       <c r="R45" s="2"/>
-    </row>
-    <row r="46" s="1" customFormat="1" spans="1:18">
+      <c r="S45" s="2"/>
+    </row>
+    <row r="46" s="1" customFormat="1" spans="1:19">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2051,8 +2101,9 @@
       <c r="P46" s="2"/>
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
-    </row>
-    <row r="47" s="1" customFormat="1" spans="1:18">
+      <c r="S46" s="2"/>
+    </row>
+    <row r="47" s="1" customFormat="1" spans="1:19">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -2071,8 +2122,9 @@
       <c r="P47" s="2"/>
       <c r="Q47" s="2"/>
       <c r="R47" s="2"/>
-    </row>
-    <row r="48" s="1" customFormat="1" spans="1:18">
+      <c r="S47" s="2"/>
+    </row>
+    <row r="48" s="1" customFormat="1" spans="1:19">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -2091,8 +2143,9 @@
       <c r="P48" s="2"/>
       <c r="Q48" s="2"/>
       <c r="R48" s="2"/>
-    </row>
-    <row r="49" s="1" customFormat="1" spans="1:18">
+      <c r="S48" s="2"/>
+    </row>
+    <row r="49" s="1" customFormat="1" spans="1:19">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -2111,8 +2164,9 @@
       <c r="P49" s="2"/>
       <c r="Q49" s="2"/>
       <c r="R49" s="2"/>
-    </row>
-    <row r="50" s="1" customFormat="1" spans="1:18">
+      <c r="S49" s="2"/>
+    </row>
+    <row r="50" s="1" customFormat="1" spans="1:19">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -2131,8 +2185,9 @@
       <c r="P50" s="2"/>
       <c r="Q50" s="2"/>
       <c r="R50" s="2"/>
-    </row>
-    <row r="51" s="1" customFormat="1" spans="1:18">
+      <c r="S50" s="2"/>
+    </row>
+    <row r="51" s="1" customFormat="1" spans="1:19">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -2151,8 +2206,9 @@
       <c r="P51" s="2"/>
       <c r="Q51" s="2"/>
       <c r="R51" s="2"/>
-    </row>
-    <row r="58" s="1" customFormat="1" spans="1:18">
+      <c r="S51" s="2"/>
+    </row>
+    <row r="58" s="1" customFormat="1" spans="1:19">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -2171,8 +2227,9 @@
       <c r="P58" s="2"/>
       <c r="Q58" s="2"/>
       <c r="R58" s="2"/>
-    </row>
-    <row r="59" s="1" customFormat="1" spans="1:18">
+      <c r="S58" s="2"/>
+    </row>
+    <row r="59" s="1" customFormat="1" spans="1:19">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -2191,8 +2248,9 @@
       <c r="P59" s="2"/>
       <c r="Q59" s="2"/>
       <c r="R59" s="2"/>
-    </row>
-    <row r="60" s="1" customFormat="1" spans="1:18">
+      <c r="S59" s="2"/>
+    </row>
+    <row r="60" s="1" customFormat="1" spans="1:19">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -2211,8 +2269,9 @@
       <c r="P60" s="2"/>
       <c r="Q60" s="2"/>
       <c r="R60" s="2"/>
-    </row>
-    <row r="61" s="1" customFormat="1" spans="1:18">
+      <c r="S60" s="2"/>
+    </row>
+    <row r="61" s="1" customFormat="1" spans="1:19">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -2231,8 +2290,9 @@
       <c r="P61" s="2"/>
       <c r="Q61" s="2"/>
       <c r="R61" s="2"/>
-    </row>
-    <row r="62" s="1" customFormat="1" spans="1:18">
+      <c r="S61" s="2"/>
+    </row>
+    <row r="62" s="1" customFormat="1" spans="1:19">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -2251,8 +2311,9 @@
       <c r="P62" s="2"/>
       <c r="Q62" s="2"/>
       <c r="R62" s="2"/>
-    </row>
-    <row r="63" s="1" customFormat="1" spans="1:18">
+      <c r="S62" s="2"/>
+    </row>
+    <row r="63" s="1" customFormat="1" spans="1:19">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -2271,8 +2332,9 @@
       <c r="P63" s="2"/>
       <c r="Q63" s="2"/>
       <c r="R63" s="2"/>
-    </row>
-    <row r="64" s="1" customFormat="1" spans="1:18">
+      <c r="S63" s="2"/>
+    </row>
+    <row r="64" s="1" customFormat="1" spans="1:19">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -2291,8 +2353,9 @@
       <c r="P64" s="2"/>
       <c r="Q64" s="2"/>
       <c r="R64" s="2"/>
-    </row>
-    <row r="65" s="1" customFormat="1" spans="1:18">
+      <c r="S64" s="2"/>
+    </row>
+    <row r="65" s="1" customFormat="1" spans="1:19">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -2311,8 +2374,9 @@
       <c r="P65" s="2"/>
       <c r="Q65" s="2"/>
       <c r="R65" s="2"/>
-    </row>
-    <row r="66" s="1" customFormat="1" spans="1:18">
+      <c r="S65" s="2"/>
+    </row>
+    <row r="66" s="1" customFormat="1" spans="1:19">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -2331,8 +2395,9 @@
       <c r="P66" s="2"/>
       <c r="Q66" s="2"/>
       <c r="R66" s="2"/>
-    </row>
-    <row r="67" s="1" customFormat="1" spans="1:18">
+      <c r="S66" s="2"/>
+    </row>
+    <row r="67" s="1" customFormat="1" spans="1:19">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -2351,8 +2416,9 @@
       <c r="P67" s="2"/>
       <c r="Q67" s="2"/>
       <c r="R67" s="2"/>
-    </row>
-    <row r="68" s="1" customFormat="1" spans="1:18">
+      <c r="S67" s="2"/>
+    </row>
+    <row r="68" s="1" customFormat="1" spans="1:19">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -2371,9 +2437,10 @@
       <c r="P68" s="2"/>
       <c r="Q68" s="2"/>
       <c r="R68" s="2"/>
+      <c r="S68" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="A2:AA66">
+  <sortState ref="A2:AB66">
     <sortCondition ref="B1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
[fix][asset] Fix column bug to upload asset
</commit_message>
<xml_diff>
--- a/api/template/network_template.xlsx
+++ b/api/template/network_template.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12375" firstSheet="1"/>
+    <workbookView windowHeight="17775" firstSheet="1"/>
   </bookViews>
   <sheets>
     <sheet name="network" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">network!$A$1:$Q$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">network!$A$1:$R$78</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+  <si>
+    <t>机房号</t>
+  </si>
   <si>
     <t>机柜</t>
   </si>
@@ -50,7 +53,7 @@
     <t>资产编号</t>
   </si>
   <si>
-    <t>采购合同号</t>
+    <t>采购合同编号</t>
   </si>
   <si>
     <t>设备名称</t>
@@ -1078,28 +1081,28 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:S68"/>
+  <dimension ref="A1:T68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="2" width="10.625" style="2" customWidth="1"/>
-    <col min="3" max="11" width="20.625" style="2" customWidth="1"/>
-    <col min="12" max="12" width="15.625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="20.625" style="2" customWidth="1"/>
-    <col min="14" max="14" width="10.625" style="2" customWidth="1"/>
-    <col min="15" max="17" width="15.625" style="2" customWidth="1"/>
-    <col min="18" max="18" width="10.625" style="2" customWidth="1"/>
-    <col min="19" max="19" width="30.625" style="2" customWidth="1"/>
-    <col min="20" max="16384" width="9" style="1"/>
+    <col min="1" max="3" width="10.625" style="2" customWidth="1"/>
+    <col min="4" max="12" width="20.625" style="2" customWidth="1"/>
+    <col min="13" max="13" width="15.625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="20.625" style="2" customWidth="1"/>
+    <col min="15" max="15" width="10.625" style="2" customWidth="1"/>
+    <col min="16" max="18" width="15.625" style="2" customWidth="1"/>
+    <col min="19" max="19" width="10.625" style="2" customWidth="1"/>
+    <col min="20" max="20" width="30.625" style="2" customWidth="1"/>
+    <col min="21" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" spans="1:19">
+    <row r="1" ht="15.75" spans="1:20">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1115,7 +1118,7 @@
       <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
@@ -1157,8 +1160,11 @@
       <c r="S1" s="4" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" s="1" customFormat="1" spans="1:19">
+      <c r="T1" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" spans="1:20">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -1176,10 +1182,11 @@
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
       <c r="Q2" s="5"/>
-      <c r="R2" s="2"/>
+      <c r="R2" s="5"/>
       <c r="S2" s="2"/>
-    </row>
-    <row r="3" s="1" customFormat="1" spans="1:19">
+      <c r="T2" s="2"/>
+    </row>
+    <row r="3" s="1" customFormat="1" spans="1:20">
       <c r="A3" s="2"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -1199,8 +1206,9 @@
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
-    </row>
-    <row r="4" s="1" customFormat="1" spans="1:19">
+      <c r="T3" s="2"/>
+    </row>
+    <row r="4" s="1" customFormat="1" spans="1:20">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -1220,8 +1228,9 @@
       <c r="Q4" s="2"/>
       <c r="R4" s="2"/>
       <c r="S4" s="2"/>
-    </row>
-    <row r="5" s="1" customFormat="1" spans="1:19">
+      <c r="T4" s="2"/>
+    </row>
+    <row r="5" s="1" customFormat="1" spans="1:20">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -1241,8 +1250,9 @@
       <c r="Q5" s="2"/>
       <c r="R5" s="2"/>
       <c r="S5" s="2"/>
-    </row>
-    <row r="6" s="1" customFormat="1" spans="1:19">
+      <c r="T5" s="2"/>
+    </row>
+    <row r="6" s="1" customFormat="1" spans="1:20">
       <c r="A6" s="2"/>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -1262,8 +1272,9 @@
       <c r="Q6" s="2"/>
       <c r="R6" s="2"/>
       <c r="S6" s="2"/>
-    </row>
-    <row r="7" s="1" customFormat="1" spans="1:19">
+      <c r="T6" s="2"/>
+    </row>
+    <row r="7" s="1" customFormat="1" spans="1:20">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -1283,8 +1294,9 @@
       <c r="Q7" s="2"/>
       <c r="R7" s="2"/>
       <c r="S7" s="2"/>
-    </row>
-    <row r="8" s="1" customFormat="1" spans="1:19">
+      <c r="T7" s="2"/>
+    </row>
+    <row r="8" s="1" customFormat="1" spans="1:20">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1304,8 +1316,9 @@
       <c r="Q8" s="2"/>
       <c r="R8" s="2"/>
       <c r="S8" s="2"/>
-    </row>
-    <row r="9" s="1" customFormat="1" spans="1:19">
+      <c r="T8" s="2"/>
+    </row>
+    <row r="9" s="1" customFormat="1" spans="1:20">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
@@ -1325,8 +1338,9 @@
       <c r="Q9" s="2"/>
       <c r="R9" s="2"/>
       <c r="S9" s="2"/>
-    </row>
-    <row r="10" s="1" customFormat="1" spans="1:19">
+      <c r="T9" s="2"/>
+    </row>
+    <row r="10" s="1" customFormat="1" spans="1:20">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -1346,8 +1360,9 @@
       <c r="Q10" s="2"/>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
-    </row>
-    <row r="11" s="1" customFormat="1" spans="1:19">
+      <c r="T10" s="2"/>
+    </row>
+    <row r="11" s="1" customFormat="1" spans="1:20">
       <c r="A11" s="2"/>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -1367,8 +1382,9 @@
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
       <c r="S11" s="2"/>
-    </row>
-    <row r="12" s="1" customFormat="1" spans="1:19">
+      <c r="T11" s="2"/>
+    </row>
+    <row r="12" s="1" customFormat="1" spans="1:20">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -1388,8 +1404,9 @@
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
       <c r="S12" s="2"/>
-    </row>
-    <row r="13" s="1" customFormat="1" spans="1:19">
+      <c r="T12" s="2"/>
+    </row>
+    <row r="13" s="1" customFormat="1" spans="1:20">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -1409,8 +1426,9 @@
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
-    </row>
-    <row r="14" s="1" customFormat="1" spans="1:19">
+      <c r="T13" s="2"/>
+    </row>
+    <row r="14" s="1" customFormat="1" spans="1:20">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1430,8 +1448,9 @@
       <c r="Q14" s="2"/>
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
-    </row>
-    <row r="15" s="1" customFormat="1" spans="1:19">
+      <c r="T14" s="2"/>
+    </row>
+    <row r="15" s="1" customFormat="1" spans="1:20">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
@@ -1451,8 +1470,9 @@
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
       <c r="S15" s="2"/>
-    </row>
-    <row r="16" s="1" customFormat="1" spans="1:19">
+      <c r="T15" s="2"/>
+    </row>
+    <row r="16" s="1" customFormat="1" spans="1:20">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -1472,8 +1492,9 @@
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
-    </row>
-    <row r="17" s="1" customFormat="1" spans="1:19">
+      <c r="T16" s="2"/>
+    </row>
+    <row r="17" s="1" customFormat="1" spans="1:20">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
@@ -1493,8 +1514,9 @@
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
       <c r="S17" s="2"/>
-    </row>
-    <row r="18" s="1" customFormat="1" spans="1:19">
+      <c r="T17" s="2"/>
+    </row>
+    <row r="18" s="1" customFormat="1" spans="1:20">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
@@ -1514,8 +1536,9 @@
       <c r="Q18" s="2"/>
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
-    </row>
-    <row r="19" s="1" customFormat="1" spans="1:19">
+      <c r="T18" s="2"/>
+    </row>
+    <row r="19" s="1" customFormat="1" spans="1:20">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
@@ -1535,8 +1558,9 @@
       <c r="Q19" s="2"/>
       <c r="R19" s="2"/>
       <c r="S19" s="2"/>
-    </row>
-    <row r="20" s="1" customFormat="1" spans="1:19">
+      <c r="T19" s="2"/>
+    </row>
+    <row r="20" s="1" customFormat="1" spans="1:20">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
@@ -1556,8 +1580,9 @@
       <c r="Q20" s="2"/>
       <c r="R20" s="2"/>
       <c r="S20" s="2"/>
-    </row>
-    <row r="21" s="1" customFormat="1" spans="1:19">
+      <c r="T20" s="2"/>
+    </row>
+    <row r="21" s="1" customFormat="1" spans="1:20">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
@@ -1577,8 +1602,9 @@
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
       <c r="S21" s="2"/>
-    </row>
-    <row r="22" s="1" customFormat="1" spans="1:19">
+      <c r="T21" s="2"/>
+    </row>
+    <row r="22" s="1" customFormat="1" spans="1:20">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
@@ -1598,8 +1624,9 @@
       <c r="Q22" s="2"/>
       <c r="R22" s="2"/>
       <c r="S22" s="2"/>
-    </row>
-    <row r="23" s="1" customFormat="1" spans="1:19">
+      <c r="T22" s="2"/>
+    </row>
+    <row r="23" s="1" customFormat="1" spans="1:20">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
@@ -1619,8 +1646,9 @@
       <c r="Q23" s="2"/>
       <c r="R23" s="2"/>
       <c r="S23" s="2"/>
-    </row>
-    <row r="24" s="1" customFormat="1" spans="1:19">
+      <c r="T23" s="2"/>
+    </row>
+    <row r="24" s="1" customFormat="1" spans="1:20">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1640,8 +1668,9 @@
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
       <c r="S24" s="2"/>
-    </row>
-    <row r="25" s="1" customFormat="1" spans="1:19">
+      <c r="T24" s="2"/>
+    </row>
+    <row r="25" s="1" customFormat="1" spans="1:20">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
@@ -1661,8 +1690,9 @@
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
       <c r="S25" s="2"/>
-    </row>
-    <row r="26" s="1" customFormat="1" spans="1:19">
+      <c r="T25" s="2"/>
+    </row>
+    <row r="26" s="1" customFormat="1" spans="1:20">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
@@ -1682,8 +1712,9 @@
       <c r="Q26" s="2"/>
       <c r="R26" s="2"/>
       <c r="S26" s="2"/>
-    </row>
-    <row r="27" s="1" customFormat="1" spans="1:19">
+      <c r="T26" s="2"/>
+    </row>
+    <row r="27" s="1" customFormat="1" spans="1:20">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -1703,8 +1734,9 @@
       <c r="Q27" s="2"/>
       <c r="R27" s="2"/>
       <c r="S27" s="2"/>
-    </row>
-    <row r="28" s="1" customFormat="1" spans="1:19">
+      <c r="T27" s="2"/>
+    </row>
+    <row r="28" s="1" customFormat="1" spans="1:20">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -1724,8 +1756,9 @@
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
       <c r="S28" s="2"/>
-    </row>
-    <row r="29" s="1" customFormat="1" spans="1:19">
+      <c r="T28" s="2"/>
+    </row>
+    <row r="29" s="1" customFormat="1" spans="1:20">
       <c r="A29" s="2"/>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1745,8 +1778,9 @@
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
       <c r="S29" s="2"/>
-    </row>
-    <row r="30" s="1" customFormat="1" spans="1:19">
+      <c r="T29" s="2"/>
+    </row>
+    <row r="30" s="1" customFormat="1" spans="1:20">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
@@ -1766,8 +1800,9 @@
       <c r="Q30" s="2"/>
       <c r="R30" s="2"/>
       <c r="S30" s="2"/>
-    </row>
-    <row r="31" s="1" customFormat="1" spans="1:19">
+      <c r="T30" s="2"/>
+    </row>
+    <row r="31" s="1" customFormat="1" spans="1:20">
       <c r="A31" s="2"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -1787,8 +1822,9 @@
       <c r="Q31" s="2"/>
       <c r="R31" s="2"/>
       <c r="S31" s="2"/>
-    </row>
-    <row r="32" s="1" customFormat="1" spans="1:19">
+      <c r="T31" s="2"/>
+    </row>
+    <row r="32" s="1" customFormat="1" spans="1:20">
       <c r="A32" s="2"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -1808,8 +1844,9 @@
       <c r="Q32" s="2"/>
       <c r="R32" s="2"/>
       <c r="S32" s="2"/>
-    </row>
-    <row r="33" s="1" customFormat="1" spans="1:19">
+      <c r="T32" s="2"/>
+    </row>
+    <row r="33" s="1" customFormat="1" spans="1:20">
       <c r="A33" s="2"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1829,8 +1866,9 @@
       <c r="Q33" s="2"/>
       <c r="R33" s="2"/>
       <c r="S33" s="2"/>
-    </row>
-    <row r="34" s="1" customFormat="1" spans="1:19">
+      <c r="T33" s="2"/>
+    </row>
+    <row r="34" s="1" customFormat="1" spans="1:20">
       <c r="A34" s="2"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -1850,8 +1888,9 @@
       <c r="Q34" s="2"/>
       <c r="R34" s="2"/>
       <c r="S34" s="2"/>
-    </row>
-    <row r="35" s="1" customFormat="1" spans="1:19">
+      <c r="T34" s="2"/>
+    </row>
+    <row r="35" s="1" customFormat="1" spans="1:20">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -1871,8 +1910,9 @@
       <c r="Q35" s="2"/>
       <c r="R35" s="2"/>
       <c r="S35" s="2"/>
-    </row>
-    <row r="36" s="1" customFormat="1" spans="1:19">
+      <c r="T35" s="2"/>
+    </row>
+    <row r="36" s="1" customFormat="1" spans="1:20">
       <c r="A36" s="2"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -1892,8 +1932,9 @@
       <c r="Q36" s="2"/>
       <c r="R36" s="2"/>
       <c r="S36" s="2"/>
-    </row>
-    <row r="37" s="1" customFormat="1" spans="1:19">
+      <c r="T36" s="2"/>
+    </row>
+    <row r="37" s="1" customFormat="1" spans="1:20">
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1913,8 +1954,9 @@
       <c r="Q37" s="2"/>
       <c r="R37" s="2"/>
       <c r="S37" s="2"/>
-    </row>
-    <row r="38" s="1" customFormat="1" spans="1:19">
+      <c r="T37" s="2"/>
+    </row>
+    <row r="38" s="1" customFormat="1" spans="1:20">
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -1934,8 +1976,9 @@
       <c r="Q38" s="2"/>
       <c r="R38" s="2"/>
       <c r="S38" s="2"/>
-    </row>
-    <row r="39" s="1" customFormat="1" spans="1:19">
+      <c r="T38" s="2"/>
+    </row>
+    <row r="39" s="1" customFormat="1" spans="1:20">
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -1955,8 +1998,9 @@
       <c r="Q39" s="2"/>
       <c r="R39" s="2"/>
       <c r="S39" s="2"/>
-    </row>
-    <row r="40" s="1" customFormat="1" spans="1:19">
+      <c r="T39" s="2"/>
+    </row>
+    <row r="40" s="1" customFormat="1" spans="1:20">
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -1976,8 +2020,9 @@
       <c r="Q40" s="2"/>
       <c r="R40" s="2"/>
       <c r="S40" s="2"/>
-    </row>
-    <row r="41" s="1" customFormat="1" spans="1:19">
+      <c r="T40" s="2"/>
+    </row>
+    <row r="41" s="1" customFormat="1" spans="1:20">
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -1997,8 +2042,9 @@
       <c r="Q41" s="2"/>
       <c r="R41" s="2"/>
       <c r="S41" s="2"/>
-    </row>
-    <row r="42" s="1" customFormat="1" spans="1:19">
+      <c r="T41" s="2"/>
+    </row>
+    <row r="42" s="1" customFormat="1" spans="1:20">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -2018,8 +2064,9 @@
       <c r="Q42" s="2"/>
       <c r="R42" s="2"/>
       <c r="S42" s="2"/>
-    </row>
-    <row r="43" s="1" customFormat="1" spans="1:19">
+      <c r="T42" s="2"/>
+    </row>
+    <row r="43" s="1" customFormat="1" spans="1:20">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -2039,8 +2086,9 @@
       <c r="Q43" s="2"/>
       <c r="R43" s="2"/>
       <c r="S43" s="2"/>
-    </row>
-    <row r="44" s="1" customFormat="1" spans="1:19">
+      <c r="T43" s="2"/>
+    </row>
+    <row r="44" s="1" customFormat="1" spans="1:20">
       <c r="A44" s="2"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -2060,8 +2108,9 @@
       <c r="Q44" s="2"/>
       <c r="R44" s="2"/>
       <c r="S44" s="2"/>
-    </row>
-    <row r="45" s="1" customFormat="1" spans="1:19">
+      <c r="T44" s="2"/>
+    </row>
+    <row r="45" s="1" customFormat="1" spans="1:20">
       <c r="A45" s="2"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -2081,8 +2130,9 @@
       <c r="Q45" s="2"/>
       <c r="R45" s="2"/>
       <c r="S45" s="2"/>
-    </row>
-    <row r="46" s="1" customFormat="1" spans="1:19">
+      <c r="T45" s="2"/>
+    </row>
+    <row r="46" s="1" customFormat="1" spans="1:20">
       <c r="A46" s="2"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2102,8 +2152,9 @@
       <c r="Q46" s="2"/>
       <c r="R46" s="2"/>
       <c r="S46" s="2"/>
-    </row>
-    <row r="47" s="1" customFormat="1" spans="1:19">
+      <c r="T46" s="2"/>
+    </row>
+    <row r="47" s="1" customFormat="1" spans="1:20">
       <c r="A47" s="2"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -2123,8 +2174,9 @@
       <c r="Q47" s="2"/>
       <c r="R47" s="2"/>
       <c r="S47" s="2"/>
-    </row>
-    <row r="48" s="1" customFormat="1" spans="1:19">
+      <c r="T47" s="2"/>
+    </row>
+    <row r="48" s="1" customFormat="1" spans="1:20">
       <c r="A48" s="2"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -2144,8 +2196,9 @@
       <c r="Q48" s="2"/>
       <c r="R48" s="2"/>
       <c r="S48" s="2"/>
-    </row>
-    <row r="49" s="1" customFormat="1" spans="1:19">
+      <c r="T48" s="2"/>
+    </row>
+    <row r="49" s="1" customFormat="1" spans="1:20">
       <c r="A49" s="2"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -2165,8 +2218,9 @@
       <c r="Q49" s="2"/>
       <c r="R49" s="2"/>
       <c r="S49" s="2"/>
-    </row>
-    <row r="50" s="1" customFormat="1" spans="1:19">
+      <c r="T49" s="2"/>
+    </row>
+    <row r="50" s="1" customFormat="1" spans="1:20">
       <c r="A50" s="2"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -2186,8 +2240,9 @@
       <c r="Q50" s="2"/>
       <c r="R50" s="2"/>
       <c r="S50" s="2"/>
-    </row>
-    <row r="51" s="1" customFormat="1" spans="1:19">
+      <c r="T50" s="2"/>
+    </row>
+    <row r="51" s="1" customFormat="1" spans="1:20">
       <c r="A51" s="2"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -2207,8 +2262,9 @@
       <c r="Q51" s="2"/>
       <c r="R51" s="2"/>
       <c r="S51" s="2"/>
-    </row>
-    <row r="58" s="1" customFormat="1" spans="1:19">
+      <c r="T51" s="2"/>
+    </row>
+    <row r="58" s="1" customFormat="1" spans="1:20">
       <c r="A58" s="2"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -2228,8 +2284,9 @@
       <c r="Q58" s="2"/>
       <c r="R58" s="2"/>
       <c r="S58" s="2"/>
-    </row>
-    <row r="59" s="1" customFormat="1" spans="1:19">
+      <c r="T58" s="2"/>
+    </row>
+    <row r="59" s="1" customFormat="1" spans="1:20">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -2249,8 +2306,9 @@
       <c r="Q59" s="2"/>
       <c r="R59" s="2"/>
       <c r="S59" s="2"/>
-    </row>
-    <row r="60" s="1" customFormat="1" spans="1:19">
+      <c r="T59" s="2"/>
+    </row>
+    <row r="60" s="1" customFormat="1" spans="1:20">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -2270,8 +2328,9 @@
       <c r="Q60" s="2"/>
       <c r="R60" s="2"/>
       <c r="S60" s="2"/>
-    </row>
-    <row r="61" s="1" customFormat="1" spans="1:19">
+      <c r="T60" s="2"/>
+    </row>
+    <row r="61" s="1" customFormat="1" spans="1:20">
       <c r="A61" s="2"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -2291,8 +2350,9 @@
       <c r="Q61" s="2"/>
       <c r="R61" s="2"/>
       <c r="S61" s="2"/>
-    </row>
-    <row r="62" s="1" customFormat="1" spans="1:19">
+      <c r="T61" s="2"/>
+    </row>
+    <row r="62" s="1" customFormat="1" spans="1:20">
       <c r="A62" s="2"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -2312,8 +2372,9 @@
       <c r="Q62" s="2"/>
       <c r="R62" s="2"/>
       <c r="S62" s="2"/>
-    </row>
-    <row r="63" s="1" customFormat="1" spans="1:19">
+      <c r="T62" s="2"/>
+    </row>
+    <row r="63" s="1" customFormat="1" spans="1:20">
       <c r="A63" s="2"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -2333,8 +2394,9 @@
       <c r="Q63" s="2"/>
       <c r="R63" s="2"/>
       <c r="S63" s="2"/>
-    </row>
-    <row r="64" s="1" customFormat="1" spans="1:19">
+      <c r="T63" s="2"/>
+    </row>
+    <row r="64" s="1" customFormat="1" spans="1:20">
       <c r="A64" s="2"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -2354,8 +2416,9 @@
       <c r="Q64" s="2"/>
       <c r="R64" s="2"/>
       <c r="S64" s="2"/>
-    </row>
-    <row r="65" s="1" customFormat="1" spans="1:19">
+      <c r="T64" s="2"/>
+    </row>
+    <row r="65" s="1" customFormat="1" spans="1:20">
       <c r="A65" s="2"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -2375,8 +2438,9 @@
       <c r="Q65" s="2"/>
       <c r="R65" s="2"/>
       <c r="S65" s="2"/>
-    </row>
-    <row r="66" s="1" customFormat="1" spans="1:19">
+      <c r="T65" s="2"/>
+    </row>
+    <row r="66" s="1" customFormat="1" spans="1:20">
       <c r="A66" s="2"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -2396,8 +2460,9 @@
       <c r="Q66" s="2"/>
       <c r="R66" s="2"/>
       <c r="S66" s="2"/>
-    </row>
-    <row r="67" s="1" customFormat="1" spans="1:19">
+      <c r="T66" s="2"/>
+    </row>
+    <row r="67" s="1" customFormat="1" spans="1:20">
       <c r="A67" s="2"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -2417,8 +2482,9 @@
       <c r="Q67" s="2"/>
       <c r="R67" s="2"/>
       <c r="S67" s="2"/>
-    </row>
-    <row r="68" s="1" customFormat="1" spans="1:19">
+      <c r="T67" s="2"/>
+    </row>
+    <row r="68" s="1" customFormat="1" spans="1:20">
       <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -2438,10 +2504,11 @@
       <c r="Q68" s="2"/>
       <c r="R68" s="2"/>
       <c r="S68" s="2"/>
+      <c r="T68" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="A2:AB66">
-    <sortCondition ref="B1"/>
+  <sortState ref="A2:AC66">
+    <sortCondition ref="C1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
[fix][asset] Fix template bug to upload asset
</commit_message>
<xml_diff>
--- a/api/template/network_template.xlsx
+++ b/api/template/network_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17775" firstSheet="1"/>
+    <workbookView windowWidth="27945" windowHeight="12375" firstSheet="1"/>
   </bookViews>
   <sheets>
     <sheet name="network" sheetId="3" r:id="rId1"/>
@@ -102,7 +102,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -113,6 +113,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="等线"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -614,137 +621,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -755,6 +762,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1086,7 +1096,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1124,65 +1134,65 @@
       <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="5" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" s="1" customFormat="1" spans="1:20">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
+      <c r="A2" s="6"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
       <c r="S2" s="2"/>
       <c r="T2" s="2"/>
     </row>

</xml_diff>